<commit_message>
Added required headers to the simulator for GET, POST and PUT. Added example in test_server excel.
</commit_message>
<xml_diff>
--- a/test_server/test_server.xlsx
+++ b/test_server/test_server.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\api-server-sim\test_server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01675978-47EF-47D9-9463-42A961FE38E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="16395" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>GET</t>
   </si>
@@ -140,11 +139,26 @@
   "lastName": "New Last Name"
 }</t>
   </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>{"rate": 1.12}</t>
+  </si>
+  <si>
+    <t>headers</t>
+  </si>
+  <si>
+    <t>./fx_rates/request_headers.json</t>
+  </si>
+  <si>
+    <t>/fx_rates/eur/usd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -208,13 +222,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -530,281 +545,335 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.06640625" customWidth="1"/>
-    <col min="4" max="4" width="15.46484375" customWidth="1"/>
-    <col min="5" max="5" width="5.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4">
-        <v>200</v>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4">
+        <v>200</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4">
-        <v>200</v>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <v>200</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="4">
+      <c r="G4" s="4">
         <v>403</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4">
         <v>201</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4">
-        <v>200</v>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4">
+        <v>200</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4">
-        <v>200</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="4">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="4">
-        <v>200</v>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="4">
+        <v>200</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="4">
         <v>404</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="H9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="4">
-        <v>200</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4">
+        <v>200</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4">
-        <v>200</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4">
+        <v>200</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4">
-        <v>200</v>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="4">
+        <v>200</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="4">
-        <v>200</v>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="4">
+        <v>200</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4">
+        <v>200</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved matching so Excel can have empty cells for query and body
</commit_message>
<xml_diff>
--- a/test_server/test_server.xlsx
+++ b/test_server/test_server.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>GET</t>
   </si>
@@ -549,7 +549,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,12 +598,8 @@
         <v>1</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="4">
         <v>200</v>
       </c>
@@ -620,12 +616,8 @@
         <v>5</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="4">
         <v>200</v>
       </c>
@@ -642,9 +634,7 @@
         <v>28</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="1" t="s">
         <v>29</v>
       </c>
@@ -667,9 +657,7 @@
       <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4">
         <v>201</v>
       </c>
@@ -686,12 +674,8 @@
         <v>7</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="4">
         <v>200</v>
       </c>
@@ -711,9 +695,7 @@
       <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="4">
         <v>200</v>
       </c>
@@ -730,12 +712,8 @@
         <v>6</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="4">
         <v>200</v>
       </c>
@@ -752,12 +730,8 @@
         <v>26</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="4">
         <v>404</v>
       </c>
@@ -774,9 +748,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
         <v>19</v>
       </c>
@@ -796,9 +768,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
         <v>20</v>
       </c>
@@ -818,12 +788,8 @@
         <v>10</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="4">
         <v>200</v>
       </c>
@@ -839,12 +805,8 @@
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="4">
         <v>200</v>
       </c>
@@ -863,12 +825,8 @@
       <c r="D14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="4">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
added acceptance tests. reorganized tests.  added linting and tsc.
</commit_message>
<xml_diff>
--- a/test_server/test_server.xlsx
+++ b/test_server/test_server.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
   <si>
     <t>GET</t>
   </si>
@@ -74,21 +75,9 @@
     <t>./entitlements/krm_operator/response.json</t>
   </si>
   <si>
-    <t>./entitlements/krr_operator/response.json</t>
-  </si>
-  <si>
-    <t>./wallets/single/response.json</t>
-  </si>
-  <si>
-    <t>./wallets/list/response.json</t>
-  </si>
-  <si>
     <t>./entitlements/krm_operator/params.json</t>
   </si>
   <si>
-    <t>./entitlements/krr_operator/params.json</t>
-  </si>
-  <si>
     <t>{ "message": "Hello World!" }</t>
   </si>
   <si>
@@ -108,9 +97,6 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>/user/login</t>
   </si>
   <si>
     <t>{
@@ -153,6 +139,63 @@
   </si>
   <si>
     <t>/fx_rates/eur/usd</t>
+  </si>
+  <si>
+    <t>/users/login</t>
+  </si>
+  <si>
+    <t>can match PUT method</t>
+  </si>
+  <si>
+    <t>can match GET method, url and return status with response</t>
+  </si>
+  <si>
+    <t>can match headers</t>
+  </si>
+  <si>
+    <t>response can be a json file</t>
+  </si>
+  <si>
+    <t>query can be a json file</t>
+  </si>
+  <si>
+    <t>headers can be a json file</t>
+  </si>
+  <si>
+    <t>/fx_rates/eur/gbp</t>
+  </si>
+  <si>
+    <t>{"Authorization": "Token _qwwersadfasdfasdf"}</t>
+  </si>
+  <si>
+    <t>{"rate": 2.00}</t>
+  </si>
+  <si>
+    <t>can match query</t>
+  </si>
+  <si>
+    <t>urls can contain numbers to create specific calls</t>
+  </si>
+  <si>
+    <t>urls can be as complex as required</t>
+  </si>
+  <si>
+    <t>can match POST method and body</t>
+  </si>
+  <si>
+    <t>can have any number of scenarios</t>
+  </si>
+  <si>
+    <t>can parse all the tabs in the Excel</t>
+  </si>
+  <si>
+    <t>{"name": "sample"}</t>
+  </si>
+  <si>
+    <t>[{"name": "sample"}, {"name": "sample2"}]</t>
+  </si>
+  <si>
+    <t>can return error codes</t>
   </si>
 </sst>
 </file>
@@ -222,14 +265,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -247,6 +286,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H12" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:H12"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="scenario" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="method" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="url" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="headers" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="body" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="query" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="status" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="response" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,296 +602,339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="57.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G4">
+        <v>403</v>
+      </c>
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4">
+      <c r="G5">
+        <v>201</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6">
         <v>200</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4">
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7">
         <v>200</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="H7" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="4">
-        <v>403</v>
-      </c>
-      <c r="H4" s="5" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <v>404</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>200</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11">
+        <v>200</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
+      <c r="H12" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4">
-        <v>201</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4">
-        <v>200</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4">
-        <v>200</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4">
-        <v>200</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4">
-        <v>404</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="4">
-        <v>200</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="4">
-        <v>200</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4">
-        <v>200</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4">
-        <v>200</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4">
-        <v>200</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved tests and reporting, linting, tsc, cspell.
</commit_message>
<xml_diff>
--- a/test_server/test_server.xlsx
+++ b/test_server/test_server.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>GET</t>
   </si>
@@ -165,9 +165,6 @@
     <t>/fx_rates/eur/gbp</t>
   </si>
   <si>
-    <t>{"Authorization": "Token _qwwersadfasdfasdf"}</t>
-  </si>
-  <si>
     <t>{"rate": 2.00}</t>
   </si>
   <si>
@@ -196,6 +193,21 @@
   </si>
   <si>
     <t>can return error codes</t>
+  </si>
+  <si>
+    <t>can match body</t>
+  </si>
+  <si>
+    <t>{
+  "username": "user.maker",
+  "password": "1235"
+}</t>
+  </si>
+  <si>
+    <t>{ "confirmationMessage": "Authorized user"}</t>
+  </si>
+  <si>
+    <t>{"Authorization": "Token TheToken"}</t>
   </si>
 </sst>
 </file>
@@ -265,10 +277,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -289,8 +303,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H12" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:H12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:H13"/>
   <tableColumns count="8">
     <tableColumn id="1" name="scenario" dataCellStyle="Normal"/>
     <tableColumn id="2" name="method" dataCellStyle="Normal"/>
@@ -602,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +629,7 @@
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" customWidth="1"/>
     <col min="8" max="8" width="57.85546875" customWidth="1"/>
   </cols>
@@ -682,7 +696,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -701,153 +715,175 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5">
-        <v>201</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
+      <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4">
+        <v>200</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
       </c>
       <c r="G6">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
       <c r="G7">
         <v>200</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
       </c>
       <c r="G8">
         <v>200</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="G9">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G10">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
       </c>
       <c r="G11">
         <v>200</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="G12">
-        <v>200</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="G13">
+        <v>200</v>
+      </c>
+      <c r="H13" t="s">
         <v>30</v>
       </c>
     </row>
@@ -864,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -902,7 +938,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -914,12 +950,12 @@
         <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -931,7 +967,7 @@
         <v>200</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delivering /calls endpoint to report server activity for successful calls. Increased minor version to 10
</commit_message>
<xml_diff>
--- a/test_server/test_server.xlsx
+++ b/test_server/test_server.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
   <si>
     <t>GET</t>
   </si>
@@ -208,6 +208,67 @@
   </si>
   <si>
     <t>{"Authorization": "Token TheToken"}</t>
+  </si>
+  <si>
+    <t>can report calls to an endpoint</t>
+  </si>
+  <si>
+    <t>/notifications/sms</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Your OTP number for Lydia App is 875987",
+    "phoneNumber": "+65 91979801"
+}</t>
+  </si>
+  <si>
+    <t>can report calls to an endpoint, example 2</t>
+  </si>
+  <si>
+    <t>/notifications/email</t>
+  </si>
+  <si>
+    <t>{
+    "receiverAddress": "receiver@lydia.io",
+    "ccAddress": "",
+    "bccAddress": "",
+    "subject": "Lydia Mobile App",
+    "body": "Please download the Lydia Mobile App"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Your OTP number for Lydia App is 875987",
+    "phoneNumber": "+65 91979801",
+    "timeStamp": "1573751636"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Your OTP number for Lydia App is 875987",
+    "phoneNumber": "+65 91979801",
+    "timeStamp": "1573751636" 
+}</t>
+  </si>
+  <si>
+    <t>can report calls</t>
+  </si>
+  <si>
+    <t>/calls/expected</t>
+  </si>
+  <si>
+    <t>{
+    "port": 3000,
+    "calls": [
+        {
+            "method": "GET",
+            "url": "/hello",
+            "headers": {},
+            "body": {},
+            "query": {}
+        }
+    ]
+}</t>
   </si>
 </sst>
 </file>
@@ -263,9 +324,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -277,19 +336,56 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -314,6 +410,23 @@
     <tableColumn id="6" name="query" dataCellStyle="Normal"/>
     <tableColumn id="7" name="status" dataCellStyle="Normal"/>
     <tableColumn id="8" name="response" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H6" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2" headerRowCellStyle="Accent6">
+  <autoFilter ref="A1:H6"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="scenario"/>
+    <tableColumn id="2" name="method"/>
+    <tableColumn id="3" name="url"/>
+    <tableColumn id="4" name="headers"/>
+    <tableColumn id="5" name="body"/>
+    <tableColumn id="6" name="query"/>
+    <tableColumn id="7" name="status"/>
+    <tableColumn id="8" name="response"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -618,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,24 +828,24 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4">
-        <v>200</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="2">
+        <v>200</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -898,41 +1011,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="8" max="8" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -970,7 +1086,72 @@
         <v>50</v>
       </c>
     </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <v>200</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <v>200</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>200</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
0.0.11 provides calls/last and flush mechanisms.
</commit_message>
<xml_diff>
--- a/test_server/test_server.xlsx
+++ b/test_server/test_server.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="http" sheetId="1" r:id="rId1"/>
+    <sheet name="tabs" sheetId="2" r:id="rId2"/>
+    <sheet name="calls" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>GET</t>
   </si>
@@ -234,13 +235,6 @@
     "bccAddress": "",
     "subject": "Lydia Mobile App",
     "body": "Please download the Lydia Mobile App"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "message": "Your OTP number for Lydia App is 875987",
-    "phoneNumber": "+65 91979801",
-    "timeStamp": "1573751636"
 }</t>
   </si>
   <si>
@@ -268,6 +262,16 @@
             "query": {}
         }
     ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "receiverAddress": "receiver@lydia.io",
+    "ccAddress": "",
+    "bccAddress": "",
+    "subject": "Lydia Mobile App",
+    "body": "Please download the Lydia Mobile App",
+    "timeStamp": "1573751636"
 }</t>
   </si>
 </sst>
@@ -357,7 +361,21 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -373,16 +391,29 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -416,8 +447,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H6" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2" headerRowCellStyle="Accent6">
-  <autoFilter ref="A1:H6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H3" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" headerRowCellStyle="Accent6">
+  <autoFilter ref="A1:H3"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="scenario"/>
+    <tableColumn id="2" name="method"/>
+    <tableColumn id="3" name="url"/>
+    <tableColumn id="4" name="headers"/>
+    <tableColumn id="5" name="body"/>
+    <tableColumn id="6" name="query"/>
+    <tableColumn id="7" name="status"/>
+    <tableColumn id="8" name="response"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:H4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1" headerRowCellStyle="Accent6">
+  <autoFilter ref="A1:H4"/>
   <tableColumns count="8">
     <tableColumn id="1" name="scenario"/>
     <tableColumn id="2" name="method"/>
@@ -1011,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,65 +1134,117 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="8" max="8" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6">
-        <v>200</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6">
+        <v>200</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
+        <v>200</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6">
-        <v>200</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="G6">
-        <v>200</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added an optional parameter to validate the api server itself against an open api 3 yaml file. It will validate only the paths documented under "server" property in yaml.
</commit_message>
<xml_diff>
--- a/test_server/test_server.xlsx
+++ b/test_server/test_server.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="http" sheetId="1" r:id="rId1"/>
     <sheet name="tabs" sheetId="2" r:id="rId2"/>
-    <sheet name="calls" sheetId="4" r:id="rId3"/>
+    <sheet name="swagger validation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,8 +25,148 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Centeno, Oscar</author>
+  </authors>
+  <commentList>
+    <comment ref="A14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Centeno, Oscar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is not included in the swagger file.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Centeno, Oscar</author>
+  </authors>
+  <commentList>
+    <comment ref="G5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Centeno, Oscar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+calling this endpoint will cause a 500 response. Swagger file validates "name" is required.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Centeno, Oscar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+calling this endpoint will cause a 500 response. Swagger file validates "id" is required for a PUT.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Centeno, Oscar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is not included in the swagger file.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Centeno, Oscar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+calling this endpoint will cause a 500 response. Swagger file validates DELETE method is not documented in the swagger file.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>GET</t>
   </si>
@@ -211,67 +351,75 @@
     <t>{"Authorization": "Token TheToken"}</t>
   </si>
   <si>
-    <t>can report calls to an endpoint</t>
-  </si>
-  <si>
-    <t>/notifications/sms</t>
+    <t>can validate an invalid response</t>
+  </si>
+  <si>
+    <t>/v1/wallets/1</t>
   </si>
   <si>
     <t>{
-    "message": "Your OTP number for Lydia App is 875987",
-    "phoneNumber": "+65 91979801"
+  "name": "sample"
 }</t>
   </si>
   <si>
-    <t>can report calls to an endpoint, example 2</t>
-  </si>
-  <si>
-    <t>/notifications/email</t>
+    <t>can validate swagger on endpoints under the server base url given un swagger file (test_server/v1/openapi.yaml)</t>
+  </si>
+  <si>
+    <t>/v1/wallets/2</t>
   </si>
   <si>
     <t>{
-    "receiverAddress": "receiver@lydia.io",
-    "ccAddress": "",
-    "bccAddress": "",
-    "subject": "Lydia Mobile App",
-    "body": "Please download the Lydia Mobile App"
+  "id": 1,
+  "name": "sample"
 }</t>
   </si>
   <si>
+    <t>/v1/wallets</t>
+  </si>
+  <si>
+    <t>{ "name": "sample"}</t>
+  </si>
+  <si>
+    <t>can validate an invalid PUT request body</t>
+  </si>
+  <si>
+    <t>can validate an invalid POST request body</t>
+  </si>
+  <si>
     <t>{
-    "message": "Your OTP number for Lydia App is 875987",
-    "phoneNumber": "+65 91979801",
-    "timeStamp": "1573751636" 
+  "id": 1,
+  "name": "sample2"
 }</t>
   </si>
   <si>
-    <t>can report calls</t>
-  </si>
-  <si>
-    <t>/calls/expected</t>
+    <t>{ "name2": "sample"}</t>
+  </si>
+  <si>
+    <t>can validate a valid POST request body</t>
   </si>
   <si>
     <t>{
-    "port": 3000,
-    "calls": [
-        {
-            "method": "GET",
-            "url": "/hello",
-            "headers": {},
-            "body": {},
-            "query": {}
-        }
-    ]
+  "name": "sample2"
 }</t>
   </si>
   <si>
+    <t>can validate a valid PUT request body</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>{"message": "Deleted!"}</t>
+  </si>
+  <si>
+    <t>can validate non documented methods</t>
+  </si>
+  <si>
+    <t>can match a DELETE method with query params</t>
+  </si>
+  <si>
     <t>{
-    "receiverAddress": "receiver@lydia.io",
-    "ccAddress": "",
-    "bccAddress": "",
-    "subject": "Lydia Mobile App",
-    "body": "Please download the Lydia Mobile App",
-    "timeStamp": "1573751636"
+  "id": "1"
 }</t>
   </si>
 </sst>
@@ -279,7 +427,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,8 +442,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +485,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -335,44 +520,85 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
       </border>
     </dxf>
@@ -430,8 +656,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H14" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="scenario" dataCellStyle="Normal"/>
     <tableColumn id="2" name="method" dataCellStyle="Normal"/>
@@ -447,7 +673,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H3" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" headerRowCellStyle="Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H3" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" headerRowCellStyle="Accent6">
   <autoFilter ref="A1:H3"/>
   <tableColumns count="8">
     <tableColumn id="1" name="scenario"/>
@@ -464,17 +690,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:H4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1" headerRowCellStyle="Accent6">
-  <autoFilter ref="A1:H4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:H8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" headerRowCellStyle="Accent6">
+  <autoFilter ref="A1:H8"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="scenario"/>
-    <tableColumn id="2" name="method"/>
-    <tableColumn id="3" name="url"/>
-    <tableColumn id="4" name="headers"/>
-    <tableColumn id="5" name="body"/>
-    <tableColumn id="6" name="query"/>
-    <tableColumn id="7" name="status"/>
-    <tableColumn id="8" name="response"/>
+    <tableColumn id="1" name="scenario" dataDxfId="8"/>
+    <tableColumn id="2" name="method" dataDxfId="7"/>
+    <tableColumn id="3" name="url" dataDxfId="6"/>
+    <tableColumn id="4" name="headers" dataDxfId="5"/>
+    <tableColumn id="5" name="body" dataDxfId="4"/>
+    <tableColumn id="6" name="query" dataDxfId="3"/>
+    <tableColumn id="7" name="status" dataDxfId="2"/>
+    <tableColumn id="8" name="response" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -776,11 +1002,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,11 +1274,34 @@
         <v>30</v>
       </c>
     </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="7">
+        <v>200</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1062,7 +1311,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,28 +1324,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1144,112 +1393,202 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" customWidth="1"/>
-    <col min="8" max="8" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="59.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>56</v>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6">
         <v>200</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>59</v>
+      <c r="H2" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>60</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6">
         <v>200</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <v>201</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <v>201</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
+        <v>200</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G4">
-        <v>200</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>65</v>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6">
+        <v>200</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="6">
+        <v>200</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>